<commit_message>
Part D in the report
</commit_message>
<xml_diff>
--- a/HW2/amazons/experiments.xlsx
+++ b/HW2/amazons/experiments.xlsx
@@ -72,24 +72,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -100,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,37 +264,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -321,22 +297,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,178 +637,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="18.375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="13.875" style="1" customWidth="1"/>
     <col min="6" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>0.5</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="5">
         <v>0.25</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="2">
@@ -844,7 +829,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3">
@@ -865,7 +850,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="4">
@@ -886,148 +871,148 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+      <c r="A19" s="10">
         <v>10</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="2">
@@ -1048,7 +1033,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="3">
@@ -1069,7 +1054,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="4">
@@ -1090,148 +1075,148 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
+      <c r="A35" s="10">
         <v>50</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="6" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="6" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="6" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="7" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="10" t="s">
+      <c r="A46" s="12"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="2">
@@ -1252,7 +1237,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="3">
@@ -1273,7 +1258,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B49" s="4">
@@ -1295,33 +1280,33 @@
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="27"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="11">
-        <v>1</v>
-      </c>
-      <c r="C52" s="11">
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
         <v>0.5</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="5">
         <v>0.25</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="2">
@@ -1342,7 +1327,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="3">
@@ -1363,7 +1348,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="4">

</xml_diff>

<commit_message>
fix for experiment 1
</commit_message>
<xml_diff>
--- a/HW2/amazons/experiments.xlsx
+++ b/HW2/amazons/experiments.xlsx
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -938,11 +938,11 @@
       <c r="A24" s="11"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -981,23 +981,23 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
       <c r="E28" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1005,10 +1005,10 @@
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
       <c r="D30" s="24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B31" s="2">
         <f>COUNTIF(B19:B30,"V")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2">
         <f>COUNTIF(C19:C30,"V")</f>
@@ -1025,11 +1025,11 @@
       </c>
       <c r="D31" s="2">
         <f>COUNTIF(D19:D30,"V")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E31" s="2">
         <f>COUNTIF(E19:E30,"V")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B32" s="3">
         <f>COUNTIF(B19:B30,"X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="3">
         <f>COUNTIF(C19:C30,"X")</f>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="D32" s="3">
         <f>COUNTIF(D19:D30,"X")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="3">
         <f>COUNTIF(E19:E30,"X")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B33" s="4">
         <f>B31/(B31+B32)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C33" s="4">
         <f>C31/(C31+C32)</f>
@@ -1067,11 +1067,11 @@
       </c>
       <c r="D33" s="4">
         <f>D31/(D31+D32)</f>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E33" s="4">
         <f>E31/(E31+E32)</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B53" s="2">
         <f>B47+B31+B15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C53" s="2">
         <f>C47+C31+C15</f>
@@ -1319,11 +1319,11 @@
       </c>
       <c r="D53" s="2">
         <f>D47+D31+D15</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E53" s="2">
         <f>E47+E31+E15</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="B54" s="3">
         <f>B48+B32+B16</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C54" s="3">
         <f>C48+C32+C16</f>
@@ -1340,11 +1340,11 @@
       </c>
       <c r="D54" s="3">
         <f>D48+D32+D16</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E54" s="3">
         <f>E48+E32+E16</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B55" s="4">
         <f>B53/(B53+B54)</f>
-        <v>0.1111111111111111</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C55" s="4">
         <f>C53/(C53+C54)</f>
@@ -1361,11 +1361,11 @@
       </c>
       <c r="D55" s="4">
         <f>D53/(D53+D54)</f>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E55" s="4">
         <f>E53/(E53+E54)</f>
-        <v>0.5</v>
+        <v>0.3888888888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more description to report for question 7. fixed a couple of issues with selective algorithm
</commit_message>
<xml_diff>
--- a/HW2/amazons/experiments.xlsx
+++ b/HW2/amazons/experiments.xlsx
@@ -9,10 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="experiment 1" sheetId="1" r:id="rId1"/>
+    <sheet name="experiment 1 Queen" sheetId="3" r:id="rId2"/>
+    <sheet name="experiment 1 Queen (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="experiment 1 Queen (3)" sheetId="5" r:id="rId4"/>
+    <sheet name="experiment 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -328,7 +332,97 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -637,15 +731,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
     <col min="2" max="5" width="13.875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,10 +773,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -689,32 +784,32 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -723,10 +818,10 @@
       <c r="A7" s="11"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="23"/>
     </row>
@@ -734,21 +829,21 @@
       <c r="A8" s="11"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="23"/>
     </row>
@@ -768,10 +863,10 @@
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -813,19 +908,19 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(B3:B14,"V")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(C3:C14,"V")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2">
         <f>COUNTIF(D3:D14,"V")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2">
         <f>COUNTIF(E3:E14,"V")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -834,19 +929,19 @@
       </c>
       <c r="B16" s="3">
         <f>COUNTIF(B3:B14,"X")</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3">
         <f>COUNTIF(C3:C14,"X")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="3">
         <f>COUNTIF(D3:D14,"X")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3">
         <f>COUNTIF(E3:E14,"X")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -855,19 +950,19 @@
       </c>
       <c r="B17" s="4">
         <f>B15/(B15+B16)</f>
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C17" s="4">
         <f>C15/(C15+C16)</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D17" s="4">
         <f>D15/(D15+D16)</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E17" s="4">
         <f>E15/(E15+E16)</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -882,10 +977,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -893,32 +988,32 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -927,10 +1022,10 @@
       <c r="A23" s="11"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="23"/>
     </row>
@@ -938,21 +1033,21 @@
       <c r="A24" s="11"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="23"/>
     </row>
@@ -960,10 +1055,10 @@
       <c r="A26" s="11"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -993,11 +1088,11 @@
       <c r="A29" s="11"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1017,19 +1112,19 @@
       </c>
       <c r="B31" s="2">
         <f>COUNTIF(B19:B30,"V")</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2">
         <f>COUNTIF(C19:C30,"V")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2">
         <f>COUNTIF(D19:D30,"V")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31" s="2">
         <f>COUNTIF(E19:E30,"V")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1038,19 +1133,19 @@
       </c>
       <c r="B32" s="3">
         <f>COUNTIF(B19:B30,"X")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C32" s="3">
         <f>COUNTIF(C19:C30,"X")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32" s="3">
         <f>COUNTIF(D19:D30,"X")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="3">
         <f>COUNTIF(E19:E30,"X")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,19 +1154,19 @@
       </c>
       <c r="B33" s="4">
         <f>B31/(B31+B32)</f>
-        <v>0.16666666666666666</v>
+        <v>1</v>
       </c>
       <c r="C33" s="4">
         <f>C31/(C31+C32)</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D33" s="4">
         <f>D31/(D31+D32)</f>
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="4">
         <f>E31/(E31+E32)</f>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1086,10 +1181,10 @@
         <v>50</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -1097,11 +1192,11 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="23"/>
     </row>
@@ -1119,10 +1214,10 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="23"/>
@@ -1131,10 +1226,10 @@
       <c r="A39" s="11"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="23"/>
     </row>
@@ -1142,21 +1237,21 @@
       <c r="A40" s="11"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="23"/>
     </row>
@@ -1221,19 +1316,19 @@
       </c>
       <c r="B47" s="2">
         <f>COUNTIF(B35:B46,"V")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2">
         <f>COUNTIF(C35:C46,"V")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2">
         <f>COUNTIF(D35:D46,"V")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E47" s="2">
         <f>COUNTIF(E35:E46,"V")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1242,19 +1337,19 @@
       </c>
       <c r="B48" s="3">
         <f>COUNTIF(B35:B46,"X")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C48" s="3">
         <f>COUNTIF(C35:C46,"X")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D48" s="3">
         <f>COUNTIF(D35:D46,"X")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" s="3">
         <f>COUNTIF(E35:E46,"X")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1263,19 +1358,19 @@
       </c>
       <c r="B49" s="4">
         <f>B47/(B47+B48)</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="C49" s="4">
         <f>C47/(C47+C48)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
         <f>D47/(D47+D48)</f>
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E49" s="4">
         <f>E47/(E47+E48)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1311,15 +1406,775 @@
       </c>
       <c r="B53" s="2">
         <f>B47+B31+B15</f>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C53" s="2">
         <f>C47+C31+C15</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D53" s="2">
         <f>D47+D31+D15</f>
+        <v>9</v>
+      </c>
+      <c r="E53" s="2">
+        <f>E47+E31+E15</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="3">
+        <f>B48+B32+B16</f>
+        <v>1</v>
+      </c>
+      <c r="C54" s="3">
+        <f>C48+C32+C16</f>
         <v>14</v>
+      </c>
+      <c r="D54" s="3">
+        <f>D48+D32+D16</f>
+        <v>9</v>
+      </c>
+      <c r="E54" s="3">
+        <f>E48+E32+E16</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="4">
+        <f>B53/(B53+B54)</f>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="C55" s="4">
+        <f>C53/(C53+C54)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D55" s="4">
+        <f>D53/(D53+D54)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="4">
+        <f>E53/(E53+E54)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"V"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"""V"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(B3:B14,"V")</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(C3:C14,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <f>COUNTIF(D3:D14,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <f>COUNTIF(E3:E14,"V")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f>COUNTIF(B3:B14,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <f>COUNTIF(C3:C14,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <f>COUNTIF(D3:D14,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <f>COUNTIF(E3:E14,"X")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <f>B15/(B15+B16)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C17" s="4">
+        <f>C15/(C15+C16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="4">
+        <f>D15/(D15+D16)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E17" s="4">
+        <f>E15/(E15+E16)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>10</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
+        <f>COUNTIF(B19:B30,"V")</f>
+        <v>6</v>
+      </c>
+      <c r="C31" s="2">
+        <f>COUNTIF(C19:C30,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f>COUNTIF(D19:D30,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f>COUNTIF(E19:E30,"V")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
+        <f>COUNTIF(B19:B30,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>COUNTIF(C19:C30,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <f>COUNTIF(D19:D30,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <f>COUNTIF(E19:E30,"X")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <f>B31/(B31+B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <f>C31/(C31+C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f>D31/(D31+D32)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="4">
+        <f>E31/(E31+E32)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>50</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2">
+        <f>COUNTIF(B35:B46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(C35:C46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <f>COUNTIF(D35:D46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f>COUNTIF(E35:E46,"V")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <f>COUNTIF(B35:B46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="C48" s="3">
+        <f>COUNTIF(C35:C46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D48" s="3">
+        <f>COUNTIF(D35:D46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E48" s="3">
+        <f>COUNTIF(E35:E46,"X")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="4">
+        <f>B47/(B47+B48)</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <f>C47/(C47+C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <f>D47/(D47+D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <f>E47/(E47+E48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2">
+        <f>B47+B31+B15</f>
+        <v>7</v>
+      </c>
+      <c r="C53" s="2">
+        <f>C47+C31+C15</f>
+        <v>3</v>
+      </c>
+      <c r="D53" s="2">
+        <f>D47+D31+D15</f>
+        <v>7</v>
       </c>
       <c r="E53" s="2">
         <f>E47+E31+E15</f>
@@ -1332,15 +2187,15 @@
       </c>
       <c r="B54" s="3">
         <f>B48+B32+B16</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C54" s="3">
         <f>C48+C32+C16</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D54" s="3">
         <f>D48+D32+D16</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E54" s="3">
         <f>E48+E32+E16</f>
@@ -1353,15 +2208,1587 @@
       </c>
       <c r="B55" s="4">
         <f>B53/(B53+B54)</f>
-        <v>0.16666666666666666</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C55" s="4">
         <f>C53/(C53+C54)</f>
-        <v>0.66666666666666663</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D55" s="4">
         <f>D53/(D53+D54)</f>
-        <v>0.77777777777777779</v>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E55" s="4">
+        <f>E53/(E53+E54)</f>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"V"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"""V"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(B3:B14,"V")</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(C3:C14,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <f>COUNTIF(D3:D14,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <f>COUNTIF(E3:E14,"V")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f>COUNTIF(B3:B14,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <f>COUNTIF(C3:C14,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <f>COUNTIF(D3:D14,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f>COUNTIF(E3:E14,"X")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <f>B15/(B15+B16)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C17" s="4">
+        <f>C15/(C15+C16)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D17" s="4">
+        <f>D15/(D15+D16)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E17" s="4">
+        <f>E15/(E15+E16)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>10</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
+        <f>COUNTIF(B19:B30,"V")</f>
+        <v>6</v>
+      </c>
+      <c r="C31" s="2">
+        <f>COUNTIF(C19:C30,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f>COUNTIF(D19:D30,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f>COUNTIF(E19:E30,"V")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
+        <f>COUNTIF(B19:B30,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>COUNTIF(C19:C30,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <f>COUNTIF(D19:D30,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <f>COUNTIF(E19:E30,"X")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <f>B31/(B31+B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <f>C31/(C31+C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f>D31/(D31+D32)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="4">
+        <f>E31/(E31+E32)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>50</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2">
+        <f>COUNTIF(B35:B46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(C35:C46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <f>COUNTIF(D35:D46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f>COUNTIF(E35:E46,"V")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <f>COUNTIF(B35:B46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="C48" s="3">
+        <f>COUNTIF(C35:C46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D48" s="3">
+        <f>COUNTIF(D35:D46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E48" s="3">
+        <f>COUNTIF(E35:E46,"X")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="4">
+        <f>B47/(B47+B48)</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <f>C47/(C47+C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <f>D47/(D47+D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <f>E47/(E47+E48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2">
+        <f>B47+B31+B15</f>
+        <v>7</v>
+      </c>
+      <c r="C53" s="2">
+        <f>C47+C31+C15</f>
+        <v>5</v>
+      </c>
+      <c r="D53" s="2">
+        <f>D47+D31+D15</f>
+        <v>8</v>
+      </c>
+      <c r="E53" s="2">
+        <f>E47+E31+E15</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="3">
+        <f>B48+B32+B16</f>
+        <v>11</v>
+      </c>
+      <c r="C54" s="3">
+        <f>C48+C32+C16</f>
+        <v>13</v>
+      </c>
+      <c r="D54" s="3">
+        <f>D48+D32+D16</f>
+        <v>10</v>
+      </c>
+      <c r="E54" s="3">
+        <f>E48+E32+E16</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="4">
+        <f>B53/(B53+B54)</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C55" s="4">
+        <f>C53/(C53+C54)</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D55" s="4">
+        <f>D53/(D53+D54)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E55" s="4">
+        <f>E53/(E53+E54)</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"V"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"""V"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(B3:B14,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(C3:C14,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <f>COUNTIF(D3:D14,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <f>COUNTIF(E3:E14,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f>COUNTIF(B3:B14,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="C16" s="3">
+        <f>COUNTIF(C3:C14,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <f>COUNTIF(D3:D14,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f>COUNTIF(E3:E14,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <f>B15/(B15+B16)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <f>C15/(C15+C16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="4">
+        <f>D15/(D15+D16)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E17" s="4">
+        <f>E15/(E15+E16)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="G18">
+        <f>AVERAGE(G15:G17)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H18">
+        <f>AVERAGE(H15:H17)</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="I18">
+        <f>AVERAGE(I15:I17)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="J18">
+        <f>AVERAGE(J15:J17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>10</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
+        <f>COUNTIF(B19:B30,"V")</f>
+        <v>6</v>
+      </c>
+      <c r="C31" s="2">
+        <f>COUNTIF(C19:C30,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f>COUNTIF(D19:D30,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f>COUNTIF(E19:E30,"V")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
+        <f>COUNTIF(B19:B30,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>COUNTIF(C19:C30,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <f>COUNTIF(D19:D30,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <f>COUNTIF(E19:E30,"X")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <f>B31/(B31+B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <f>C31/(C31+C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f>D31/(D31+D32)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="4">
+        <f>E31/(E31+E32)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>50</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2">
+        <f>COUNTIF(B35:B46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(C35:C46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <f>COUNTIF(D35:D46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f>COUNTIF(E35:E46,"V")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <f>COUNTIF(B35:B46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="C48" s="3">
+        <f>COUNTIF(C35:C46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="D48" s="3">
+        <f>COUNTIF(D35:D46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E48" s="3">
+        <f>COUNTIF(E35:E46,"X")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="4">
+        <f>B47/(B47+B48)</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <f>C47/(C47+C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <f>D47/(D47+D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <f>E47/(E47+E48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2">
+        <f>B47+B31+B15</f>
+        <v>6</v>
+      </c>
+      <c r="C53" s="2">
+        <f>C47+C31+C15</f>
+        <v>3</v>
+      </c>
+      <c r="D53" s="2">
+        <f>D47+D31+D15</f>
+        <v>8</v>
+      </c>
+      <c r="E53" s="2">
+        <f>E47+E31+E15</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="3">
+        <f>B48+B32+B16</f>
+        <v>12</v>
+      </c>
+      <c r="C54" s="3">
+        <f>C48+C32+C16</f>
+        <v>15</v>
+      </c>
+      <c r="D54" s="3">
+        <f>D48+D32+D16</f>
+        <v>10</v>
+      </c>
+      <c r="E54" s="3">
+        <f>E48+E32+E16</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="4">
+        <f>B53/(B53+B54)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C55" s="4">
+        <f>C53/(C53+C54)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D55" s="4">
+        <f>D53/(D53+D54)</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E55" s="4">
         <f>E53/(E53+E54)</f>
@@ -1390,4 +3817,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished experiment 1, added experiment 2 table and fixed a bug in get_w(k)
</commit_message>
<xml_diff>
--- a/HW2/amazons/experiments.xlsx
+++ b/HW2/amazons/experiments.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="experiment 1 Queen (1)" sheetId="3" r:id="rId1"/>
     <sheet name="experiment 1 Queen (2)" sheetId="4" r:id="rId2"/>
     <sheet name="experiment 1 Queen (3)" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
-    <sheet name="experiment 2" sheetId="2" r:id="rId5"/>
+    <sheet name="experiment 1 Queen (4)" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="Experiment 2" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="14">
   <si>
     <t>simple</t>
   </si>
@@ -55,6 +56,21 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Upgraded simple</t>
+  </si>
+  <si>
+    <t>Selective Alpha Beta (k)</t>
+  </si>
+  <si>
+    <t>Upgraded Selective Alpha Beta</t>
   </si>
 </sst>
 </file>
@@ -345,7 +361,457 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -864,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -1317,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="23"/>
@@ -1329,7 +1795,7 @@
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="24"/>
     </row>
@@ -1341,7 +1807,7 @@
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1453,15 +1919,15 @@
       </c>
       <c r="C47" s="3">
         <f>COUNTIF(C35:C46,"V")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="3">
         <f>COUNTIF(D35:D46,"V")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="3">
         <f>COUNTIF(E35:E46,"V")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1474,15 +1940,15 @@
       </c>
       <c r="C48" s="4">
         <f>COUNTIF(C35:C46,"X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48" s="4">
         <f>COUNTIF(D35:D46,"X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" s="4">
         <f>COUNTIF(E35:E46,"X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1495,15 +1961,15 @@
       </c>
       <c r="C49" s="5">
         <f>C47/(C47+C48)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D49" s="5">
         <f>D47/(D47+D48)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E49" s="5">
         <f>E47/(E47+E48)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1543,15 +2009,15 @@
       </c>
       <c r="C53" s="3">
         <f>C47+C31+C15</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D53" s="3">
         <f>D47+D31+D15</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E53" s="3">
         <f>E47+E31+E15</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1564,15 +2030,15 @@
       </c>
       <c r="C54" s="4">
         <f>C48+C32+C16</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D54" s="4">
         <f>D48+D32+D16</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E54" s="4">
         <f>E48+E32+E16</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1585,15 +2051,15 @@
       </c>
       <c r="C55" s="5">
         <f>C53/(C53+C54)</f>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D55" s="5">
         <f>D53/(D53+D54)</f>
-        <v>0.33333333333333331</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="E55" s="5">
         <f>E53/(E53+E54)</f>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
   </sheetData>
@@ -1605,13 +2071,13 @@
     <mergeCell ref="A51:E51"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="3" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2365,13 +2831,13 @@
     <mergeCell ref="A51:E51"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2382,10 +2848,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2633,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>7</v>
       </c>
@@ -2666,7 +3132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -2689,7 +3155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>10</v>
       </c>
@@ -2702,7 +3168,7 @@
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="24" t="s">
         <v>1</v>
@@ -2725,7 +3191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="24" t="s">
         <v>2</v>
@@ -2748,7 +3214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="24" t="s">
         <v>2</v>
@@ -2772,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
@@ -2799,7 +3265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24" t="s">
@@ -2809,8 +3275,24 @@
       <c r="E24" s="24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <f>G23/SUM(G23:J23)</f>
+        <v>0.25714285714285717</v>
+      </c>
+      <c r="H24">
+        <f>H23/SUM(G23:J23)</f>
+        <v>0.34285714285714286</v>
+      </c>
+      <c r="I24">
+        <f>I23/SUM(G23:J23)</f>
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="J24">
+        <f>J23/SUM(G23:J23)</f>
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="24" t="s">
         <v>2</v>
@@ -2821,7 +3303,7 @@
       </c>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="24"/>
       <c r="C26" s="24" t="s">
@@ -2831,8 +3313,23 @@
         <v>1</v>
       </c>
       <c r="E26" s="24"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -2842,8 +3339,23 @@
       <c r="E27" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="24" t="s">
         <v>2</v>
@@ -2853,8 +3365,23 @@
       <c r="E28" s="24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>6</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
@@ -2864,8 +3391,24 @@
       <c r="E29" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f>G28/SUM(G28:J28)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H29">
+        <f>H28/SUM(G28:J28)</f>
+        <v>0.4</v>
+      </c>
+      <c r="I29">
+        <f>I28/SUM(G28:J28)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J29">
+        <f>J28/SUM(G28:J28)</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -2876,7 +3419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>5</v>
       </c>
@@ -2897,7 +3440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>6</v>
       </c>
@@ -2916,6 +3459,18 @@
       <c r="E32" s="4">
         <f>COUNTIF(E19:E30,"X")</f>
         <v>3</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2987,7 +3542,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -2996,7 +3551,7 @@
       <c r="A39" s="12"/>
       <c r="B39" s="24"/>
       <c r="C39" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>1</v>
@@ -3007,7 +3562,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="24"/>
       <c r="C40" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24" t="s">
@@ -3029,7 +3584,7 @@
       <c r="A42" s="12"/>
       <c r="B42" s="24"/>
       <c r="C42" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>1</v>
@@ -3062,7 +3617,7 @@
       <c r="A45" s="12"/>
       <c r="B45" s="24"/>
       <c r="C45" s="24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="24" t="s">
@@ -3090,7 +3645,7 @@
       </c>
       <c r="C47" s="3">
         <f>COUNTIF(C35:C46,"V")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D47" s="3">
         <f>COUNTIF(D35:D46,"V")</f>
@@ -3111,7 +3666,7 @@
       </c>
       <c r="C48" s="4">
         <f>COUNTIF(C35:C46,"X")</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D48" s="4">
         <f>COUNTIF(D35:D46,"X")</f>
@@ -3132,7 +3687,7 @@
       </c>
       <c r="C49" s="5">
         <f>C47/(C47+C48)</f>
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D49" s="5">
         <f>D47/(D47+D48)</f>
@@ -3180,7 +3735,7 @@
       </c>
       <c r="C53" s="3">
         <f>C47+C31+C15</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D53" s="3">
         <f>D47+D31+D15</f>
@@ -3201,7 +3756,7 @@
       </c>
       <c r="C54" s="4">
         <f>C48+C32+C16</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D54" s="4">
         <f>D48+D32+D16</f>
@@ -3222,7 +3777,7 @@
       </c>
       <c r="C55" s="5">
         <f>C53/(C53+C54)</f>
-        <v>0.3888888888888889</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D55" s="5">
         <f>D53/(D53+D54)</f>
@@ -3242,13 +3797,13 @@
     <mergeCell ref="A51:E51"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46 H14:I14">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="3" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3259,16 +3814,787 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F27"/>
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E55" sqref="A1:E55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.125" style="2" customWidth="1"/>
+    <col min="2" max="5" width="13.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <f>COUNTIF(B3:B14,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <f>COUNTIF(C3:C14,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(D3:D14,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <f>COUNTIF(E3:E14,"V")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <f>COUNTIF(B3:B14,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="4">
+        <f>COUNTIF(C3:C14,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <f>COUNTIF(D3:D14,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="E16" s="4">
+        <f>COUNTIF(E3:E14,"X")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5">
+        <f>B15/(B15+B16)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C15/(C15+C16)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D17" s="5">
+        <f>D15/(D15+D16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="5">
+        <f>E15/(E15+E16)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>10</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="24"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="24"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3">
+        <f>COUNTIF(B19:B30,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <f>COUNTIF(C19:C30,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <f>COUNTIF(D19:D30,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="E31" s="3">
+        <f>COUNTIF(E19:E30,"V")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4">
+        <f>COUNTIF(B19:B30,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="C32" s="4">
+        <f>COUNTIF(C19:C30,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <f>COUNTIF(D19:D30,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="4">
+        <f>COUNTIF(E19:E30,"X")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="5">
+        <f>B31/(B31+B32)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C33" s="5">
+        <f>C31/(C31+C32)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33" s="5">
+        <f>D31/(D31+D32)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E33" s="5">
+        <f>E31/(E31+E32)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="11">
+        <v>50</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3">
+        <f>COUNTIF(B35:B46,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="C47" s="3">
+        <f>COUNTIF(C35:C46,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="D47" s="3">
+        <f>COUNTIF(D35:D46,"V")</f>
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <f>COUNTIF(E35:E46,"V")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="4">
+        <f>COUNTIF(B35:B46,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="C48" s="4">
+        <f>COUNTIF(C35:C46,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <f>COUNTIF(D35:D46,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="E48" s="4">
+        <f>COUNTIF(E35:E46,"X")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="5">
+        <f>B47/(B47+B48)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C49" s="5">
+        <f>C47/(C47+C48)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D49" s="5">
+        <f>D47/(D47+D48)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E49" s="5">
+        <f>E47/(E47+E48)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D52" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="3">
+        <f>B47+B31+B15</f>
+        <v>8</v>
+      </c>
+      <c r="C53" s="3">
+        <f>C47+C31+C15</f>
+        <v>11</v>
+      </c>
+      <c r="D53" s="3">
+        <f>D47+D31+D15</f>
+        <v>9</v>
+      </c>
+      <c r="E53" s="3">
+        <f>E47+E31+E15</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="4">
+        <f>B48+B32+B16</f>
+        <v>10</v>
+      </c>
+      <c r="C54" s="4">
+        <f>C48+C32+C16</f>
+        <v>7</v>
+      </c>
+      <c r="D54" s="4">
+        <f>D48+D32+D16</f>
+        <v>9</v>
+      </c>
+      <c r="E54" s="4">
+        <f>E48+E32+E16</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="5">
+        <f>B53/(B53+B54)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C55" s="5">
+        <f>C53/(C53+C54)</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="D55" s="5">
+        <f>D53/(D53+D54)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="5">
+        <f>E53/(E53+E54)</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E14 B35:E46 B19:E30">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"V"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"""V"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="A32:H36"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="S1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>1</v>
       </c>
@@ -3284,8 +4610,38 @@
       <c r="F3" s="6">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.75</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0.75</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -3294,8 +4650,23 @@
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="23"/>
+      <c r="J4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="24" t="s">
         <v>2</v>
       </c>
@@ -3304,8 +4675,27 @@
         <v>1</v>
       </c>
       <c r="E5" s="24"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="24"/>
+      <c r="J5" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="R5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
@@ -3314,31 +4704,79 @@
       <c r="E6" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="24" t="s">
-        <v>1</v>
-      </c>
+      <c r="F6" s="24"/>
+      <c r="J6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="24"/>
+      <c r="R6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="24"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="24"/>
+      <c r="J7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="24"/>
-      <c r="C9" t="s">
+      <c r="C9" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -3346,8 +4784,22 @@
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
         <v>1</v>
@@ -3357,41 +4809,99 @@
         <v>2</v>
       </c>
       <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
-        <v>1</v>
-      </c>
+      <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J12" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="R12" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="24"/>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="24" t="s">
         <v>2</v>
       </c>
@@ -3399,139 +4909,403 @@
         <v>1</v>
       </c>
       <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="V14" s="24"/>
+    </row>
+    <row r="15" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
-      <c r="D15" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="25"/>
-      <c r="F15" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
+      <c r="F15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="J16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="23"/>
+      <c r="R16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="23"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E19" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="U18" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" s="24"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="J20" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="V23" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f>COUNTIF(B4:B24,"V")</f>
         <v>2</v>
       </c>
       <c r="C25" s="3">
         <f>COUNTIF(C4:C24,"V")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="3">
         <f>COUNTIF(D4:D24,"V")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="3">
         <f>COUNTIF(E4:E24,"V")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" s="3">
         <f>COUNTIF(F4:F24,"V")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <f>COUNTIF(J4:J24,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="K25" s="3">
+        <f>COUNTIF(K4:K24,"V")</f>
+        <v>5</v>
+      </c>
+      <c r="L25" s="3">
+        <f>COUNTIF(L4:L24,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="M25" s="3">
+        <f>COUNTIF(M4:M24,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="N25" s="3">
+        <f>COUNTIF(N4:N24,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="R25" s="3">
+        <f>COUNTIF(R4:R24,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="S25" s="3">
+        <f>COUNTIF(S4:S24,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="3">
+        <f>COUNTIF(T4:T24,"V")</f>
+        <v>2</v>
+      </c>
+      <c r="U25" s="3">
+        <f>COUNTIF(U4:U24,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="V25" s="3">
+        <f>COUNTIF(V4:V24,"V")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <f>COUNTIF(B4:B24,"X")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" s="4">
         <f>COUNTIF(C4:C24,"X")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="4">
         <f>COUNTIF(D4:D24,"X")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="4">
         <f>COUNTIF(E4:E24,"X")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4">
         <f>COUNTIF(F4:F24,"X")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <f>COUNTIF(J4:J24,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="K26" s="4">
+        <f>COUNTIF(K4:K24,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="L26" s="4">
+        <f>COUNTIF(L4:L24,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="M26" s="4">
+        <f>COUNTIF(M4:M24,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="N26" s="4">
+        <f>COUNTIF(N4:N24,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="R26" s="4">
+        <f>COUNTIF(R4:R24,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="S26" s="4">
+        <f>COUNTIF(S4:S24,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="4">
+        <f>COUNTIF(T4:T24,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="U26" s="4">
+        <f>COUNTIF(U4:U24,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="V26" s="4">
+        <f>COUNTIF(V4:V24,"X")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <f>B25/(B25+B26)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C27" s="5">
         <f>C25/(C25+C26)</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D27" s="5">
         <f>D25/(D25+D26)</f>
@@ -3539,59 +5313,836 @@
       </c>
       <c r="E27" s="5">
         <f>E25/(E25+E26)</f>
-        <v>0.75</v>
-      </c>
-      <c r="F27" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F27" s="5" t="e">
         <f>F25/(F25+F26)</f>
-        <v>0.75</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" s="5">
+        <f>J25/(J25+J26)</f>
+        <v>0.625</v>
+      </c>
+      <c r="K27" s="5">
+        <f>K25/(K25+K26)</f>
+        <v>0.625</v>
+      </c>
+      <c r="L27" s="5">
+        <f>L25/(L25+L26)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M27" s="5">
+        <f>M25/(M25+M26)</f>
+        <v>0.5</v>
+      </c>
+      <c r="N27" s="5">
+        <f>N25/(N25+N26)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R27" s="5">
+        <f>R25/(R25+R26)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S27" s="5" t="e">
+        <f>S25/(S25+S26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T27" s="5">
+        <f>T25/(T25+T26)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U27" s="5">
+        <f>U25/(U25+U26)</f>
+        <v>0.5</v>
+      </c>
+      <c r="V27" s="5">
+        <f>V25/(V25+V26)</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:B15 D7:F11 C4:E6 C10:C11 E12:F15">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+  <conditionalFormatting sqref="J4:N24">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+  <conditionalFormatting sqref="B4:F24">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+  <conditionalFormatting sqref="R4:V24">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"""V"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>"V"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"""V"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:E24">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.125" style="2" customWidth="1"/>
+    <col min="2" max="5" width="27.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="13" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <f>COUNTIF(B3:B14,"V")</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <f>COUNTIF(C3:C14,"V")</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(D3:D14,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <f>COUNTIF(E3:E14,"V")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <f>COUNTIF(B3:B14,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <f>COUNTIF(C3:C14,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <f>COUNTIF(D3:D14,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <f>COUNTIF(E3:E14,"X")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5">
+        <f>B15/(B15+B16)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C15/(C15+C16)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D17" s="5">
+        <f>D15/(D15+D16)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E17" s="5">
+        <f>E15/(E15+E16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>10</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="24"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3">
+        <f>COUNTIF(B19:B30,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="C31" s="3">
+        <f>COUNTIF(C19:C30,"V")</f>
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <f>COUNTIF(D19:D30,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <f>COUNTIF(E19:E30,"V")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4">
+        <f>COUNTIF(B19:B30,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="C32" s="4">
+        <f>COUNTIF(C19:C30,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <f>COUNTIF(D19:D30,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E32" s="4">
+        <f>COUNTIF(E19:E30,"X")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="5">
+        <f>B31/(B31+B32)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="5">
+        <f>C31/(C31+C32)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33" s="5">
+        <f>D31/(D31+D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <f>E31/(E31+E32)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="11">
+        <v>50</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3">
+        <f>COUNTIF(B35:B46,"V")</f>
+        <v>3</v>
+      </c>
+      <c r="C47" s="3">
+        <f>COUNTIF(C35:C46,"V")</f>
+        <v>6</v>
+      </c>
+      <c r="D47" s="3">
+        <f>COUNTIF(D35:D46,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <f>COUNTIF(E35:E46,"V")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="4">
+        <f>COUNTIF(B35:B46,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="C48" s="4">
+        <f>COUNTIF(C35:C46,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <f>COUNTIF(D35:D46,"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E48" s="4">
+        <f>COUNTIF(E35:E46,"X")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="5">
+        <f>B47/(B47+B48)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="5">
+        <f>C47/(C47+C48)</f>
+        <v>1</v>
+      </c>
+      <c r="D49" s="5">
+        <f>D47/(D47+D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="5">
+        <f>E47/(E47+E48)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="3">
+        <f>B47+B31+B15</f>
+        <v>7</v>
+      </c>
+      <c r="C53" s="3">
+        <f>C47+C31+C15</f>
+        <v>11</v>
+      </c>
+      <c r="D53" s="3">
+        <f>D47+D31+D15</f>
+        <v>4</v>
+      </c>
+      <c r="E53" s="3">
+        <f>E47+E31+E15</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="4">
+        <f>B48+B32+B16</f>
+        <v>11</v>
+      </c>
+      <c r="C54" s="4">
+        <f>C48+C32+C16</f>
+        <v>7</v>
+      </c>
+      <c r="D54" s="4">
+        <f>D48+D32+D16</f>
+        <v>14</v>
+      </c>
+      <c r="E54" s="4">
+        <f>E48+E32+E16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="5">
+        <f>B53/(B53+B54)</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C55" s="5">
+        <f>C53/(C53+C54)</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="D55" s="5">
+        <f>D53/(D53+D54)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E55" s="5">
+        <f>E53/(E53+E54)</f>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A51:E51"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E14 B19:E30 B35:E46">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
@@ -3603,19 +6154,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>